<commit_message>
Modification de la Documentation_Technique
</commit_message>
<xml_diff>
--- a/Diagramm de Gantt V3.xlsx
+++ b/Diagramm de Gantt V3.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Admin\Desktop\TPI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8265"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Feuille 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>OneWayTicket</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>Création et structures de la documentation</t>
   </si>
@@ -55,32 +60,38 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="20.0"/>
+      <sz val="20"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -94,6 +105,18 @@
         <bgColor rgb="FF4A86E8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor rgb="FF4A86E8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -101,6 +124,7 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -111,6 +135,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -123,6 +148,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -137,103 +163,376 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="40.43"/>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21.0" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2">
+        <v>42122</v>
+      </c>
+      <c r="C1" s="2">
+        <v>42123</v>
+      </c>
+      <c r="D1" s="2">
+        <v>42124</v>
+      </c>
+      <c r="E1" s="2">
+        <v>42129</v>
+      </c>
+      <c r="F1" s="2">
+        <v>42130</v>
+      </c>
+      <c r="G1" s="2">
+        <v>42131</v>
+      </c>
+      <c r="H1" s="3">
+        <v>42132</v>
+      </c>
+      <c r="I1" s="2">
+        <v>42136</v>
+      </c>
+      <c r="J1" s="2">
+        <v>42137</v>
+      </c>
+      <c r="K1" s="4">
+        <v>42139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
-        <v>42122.0</v>
-      </c>
-      <c r="C1" s="2">
-        <v>42123.0</v>
-      </c>
-      <c r="D1" s="2">
-        <v>42124.0</v>
-      </c>
-      <c r="E1" s="2">
-        <v>42129.0</v>
-      </c>
-      <c r="F1" s="2">
-        <v>42130.0</v>
-      </c>
-      <c r="G1" s="2">
-        <v>42131.0</v>
-      </c>
-      <c r="H1" s="3">
-        <v>42132.0</v>
-      </c>
-      <c r="I1" s="2">
-        <v>42136.0</v>
-      </c>
-      <c r="J1" s="2">
-        <v>42137.0</v>
-      </c>
-      <c r="K1" s="4">
-        <v>42139.0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
@@ -244,9 +543,9 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
@@ -259,9 +558,9 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="6"/>
@@ -274,9 +573,9 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="6"/>
@@ -289,9 +588,9 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -304,9 +603,9 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -319,9 +618,9 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -334,9 +633,9 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -349,9 +648,9 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -364,9 +663,9 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -379,9 +678,9 @@
       <c r="J11" s="10"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -394,9 +693,9 @@
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -409,7 +708,220 @@
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
     </row>
+    <row r="15" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3">
+        <v>42122</v>
+      </c>
+      <c r="C15" s="3">
+        <v>42123</v>
+      </c>
+      <c r="D15" s="3">
+        <v>42124</v>
+      </c>
+      <c r="E15" s="3">
+        <v>42129</v>
+      </c>
+      <c r="F15" s="3">
+        <v>42130</v>
+      </c>
+      <c r="G15" s="3">
+        <v>42131</v>
+      </c>
+      <c r="H15" s="3">
+        <v>42132</v>
+      </c>
+      <c r="I15" s="3">
+        <v>42136</v>
+      </c>
+      <c r="J15" s="3">
+        <v>42137</v>
+      </c>
+      <c r="K15" s="4">
+        <v>42139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="9"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="17"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>